<commit_message>
Removed target date details
</commit_message>
<xml_diff>
--- a/Oracle - CCC AWS Inventory - DBA Team Only.xlsx
+++ b/Oracle - CCC AWS Inventory - DBA Team Only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mludusan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elai\CCC\Live\Database Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1D01B3-6913-4400-A737-16BC079C7CF0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC365E4-FB28-4332-8313-1E72C9259A6A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18792" windowHeight="7932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databases" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="130">
   <si>
     <t>Env</t>
   </si>
@@ -372,12 +372,6 @@
   </si>
   <si>
     <t>1500 - 15000</t>
-  </si>
-  <si>
-    <t>Target Date</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>Run</t>
@@ -580,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,15 +614,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -640,9 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -979,47 +961,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="64.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="4" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -1041,12 +1022,9 @@
       <c r="G4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1067,12 +1045,9 @@
       <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
@@ -1091,12 +1066,9 @@
       <c r="G6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
       <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
@@ -1115,12 +1087,9 @@
       <c r="G7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
       <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
@@ -1139,12 +1108,9 @@
       <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1165,12 +1131,9 @@
       <c r="G9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
       <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
@@ -1189,12 +1152,9 @@
       <c r="G10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1213,12 +1173,9 @@
       <c r="G11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1239,12 +1196,9 @@
       <c r="G12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
       <c r="B13" s="12" t="s">
         <v>38</v>
       </c>
@@ -1263,12 +1217,9 @@
       <c r="G13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
       <c r="B14" s="12" t="s">
         <v>45</v>
       </c>
@@ -1287,12 +1238,9 @@
       <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>93</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1313,12 +1261,9 @@
       <c r="G15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
       <c r="B16" s="12" t="s">
         <v>38</v>
       </c>
@@ -1337,12 +1282,9 @@
       <c r="G16" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
       <c r="B17" s="12" t="s">
         <v>45</v>
       </c>
@@ -1361,11 +1303,8 @@
       <c r="G17" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>61</v>
       </c>
@@ -1387,11 +1326,8 @@
       <c r="G18" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>66</v>
       </c>
@@ -1413,21 +1349,18 @@
       <c r="G19" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+    </row>
+    <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="13" t="s">
@@ -1436,22 +1369,19 @@
       <c r="F20" s="13">
         <v>1541</v>
       </c>
-      <c r="G20" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="22">
-        <v>43540</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="20" t="s">
+      <c r="G20" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="17" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="13" t="s">
@@ -1460,15 +1390,12 @@
       <c r="F21" s="13">
         <v>1530</v>
       </c>
-      <c r="G21" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="22">
-        <v>43540</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="G21" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
       <c r="B22" s="12" t="s">
         <v>70</v>
       </c>
@@ -1487,12 +1414,9 @@
       <c r="G22" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23" s="12" t="s">
         <v>70</v>
       </c>
@@ -1511,12 +1435,9 @@
       <c r="G23" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="17">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
       <c r="B24" s="12" t="s">
         <v>70</v>
       </c>
@@ -1535,12 +1456,9 @@
       <c r="G24" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
       <c r="B25" s="12" t="s">
         <v>70</v>
       </c>
@@ -1559,12 +1477,9 @@
       <c r="G25" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H25" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>89</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -1585,12 +1500,9 @@
       <c r="G26" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H26" s="17">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
       <c r="B27" s="12" t="s">
         <v>90</v>
       </c>
@@ -1609,12 +1521,9 @@
       <c r="G27" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="H27" s="17">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
       <c r="B28" s="12" t="s">
         <v>90</v>
       </c>
@@ -1633,60 +1542,51 @@
       <c r="G28" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="H28" s="17">
-        <v>43553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>121</v>
-      </c>
       <c r="C29" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F29" s="14">
         <v>1521</v>
       </c>
       <c r="G29" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>123</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="F30" s="14">
         <v>1521</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1710,49 +1610,49 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="str">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="str">
         <f>Databases!$A$2</f>
         <v>Last Update: 02/21/2019, By Evan Lai</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
-      <c r="F4" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1765,21 +1665,21 @@
       <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>111</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="23" t="s">
         <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1788,7 +1688,7 @@
       <c r="D6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F6" s="2">
@@ -1798,18 +1698,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F7" s="2">
@@ -1819,11 +1719,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="23" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1832,7 +1732,7 @@
       <c r="D8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F8" s="2">
@@ -1842,18 +1742,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F9" s="2">
@@ -1863,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1876,7 +1776,7 @@
       <c r="D10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F10" s="2">
@@ -1886,7 +1786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -1899,7 +1799,7 @@
       <c r="D11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F11" s="2">
@@ -1909,7 +1809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -1922,7 +1822,7 @@
       <c r="D12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F12" s="2">
@@ -1932,7 +1832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>89</v>
       </c>
@@ -1945,7 +1845,7 @@
       <c r="D13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F13" s="2">

</xml_diff>